<commit_message>
Update Excel files with new string resource
</commit_message>
<xml_diff>
--- a/ErgoLux/localization/Arabic (ar) translation.xlsx
+++ b/ErgoLux/localization/Arabic (ar) translation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44993843R\source\repos\ErgoLux\ErgoLux\localization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB0A99F-80EF-4394-B54D-87517DD812CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AE1844-4B46-452D-BB23-785A5DE18E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51C6AD1F-7C4A-41E1-BFD1-D5AAE4E918C7}"/>
   </bookViews>
   <sheets>
     <sheet name="ar" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="403">
   <si>
     <t>Key</t>
   </si>
@@ -1261,6 +1261,15 @@
   </si>
   <si>
     <t>Plots' context menu</t>
+  </si>
+  <si>
+    <t>strWindowPos</t>
+  </si>
+  <si>
+    <t>Remember window position and size on startup</t>
+  </si>
+  <si>
+    <t>In "settings" form, tab "User interface"</t>
   </si>
 </sst>
 </file>
@@ -1350,10 +1359,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:F203" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="B2:F203" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:F169">
-    <sortCondition ref="C2:C169"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0DD7C0AF-0A3F-45E4-9CF3-D3036D280B58}" name="Tabla13" displayName="Tabla13" ref="B2:F204" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="B2:F204" xr:uid="{64291C3F-0D0C-4C57-A011-4795D69358B3}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:F170">
+    <sortCondition ref="C2:C170"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="4" xr3:uid="{62D99807-3CD1-4982-BA4E-EA86034C60FF}" name="File" dataDxfId="4"/>
@@ -1663,7 +1672,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99272ECF-2233-463E-857F-E2B1C41A5F55}">
-  <dimension ref="B2:AH332"/>
+  <dimension ref="B2:AH333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1671,7 +1680,7 @@
   <cols>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
     <col min="5" max="5" width="55.5703125" customWidth="1"/>
     <col min="6" max="6" width="56.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
@@ -2045,7 +2054,9 @@
       <c r="C25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>402</v>
+      </c>
       <c r="E25" s="3" t="s">
         <v>19</v>
       </c>
@@ -2129,55 +2140,57 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -2186,11 +2199,11 @@
         <v>392</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F36" s="1"/>
     </row>
@@ -2199,11 +2212,11 @@
         <v>392</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F37" s="1"/>
     </row>
@@ -2212,11 +2225,11 @@
         <v>392</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F38" s="1"/>
     </row>
@@ -2225,11 +2238,11 @@
         <v>392</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -2238,11 +2251,11 @@
         <v>392</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -2251,11 +2264,11 @@
         <v>392</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -2264,11 +2277,11 @@
         <v>392</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F42" s="1"/>
     </row>
@@ -2277,11 +2290,11 @@
         <v>392</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>176</v>
+        <v>42</v>
       </c>
       <c r="F43" s="1"/>
     </row>
@@ -2290,11 +2303,11 @@
         <v>392</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="F44" s="1"/>
     </row>
@@ -2303,11 +2316,11 @@
         <v>392</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F45" s="1"/>
     </row>
@@ -2316,11 +2329,11 @@
         <v>392</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F46" s="1"/>
     </row>
@@ -2329,11 +2342,11 @@
         <v>392</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3" t="s">
-        <v>177</v>
+        <v>48</v>
       </c>
       <c r="F47" s="1"/>
     </row>
@@ -2342,11 +2355,11 @@
         <v>392</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F48" s="1"/>
     </row>
@@ -2355,11 +2368,11 @@
         <v>392</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F49" s="1"/>
     </row>
@@ -2368,11 +2381,11 @@
         <v>392</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>44</v>
+        <v>179</v>
       </c>
       <c r="F50" s="1"/>
     </row>
@@ -2381,11 +2394,11 @@
         <v>392</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="F51" s="1"/>
     </row>
@@ -2394,11 +2407,11 @@
         <v>392</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3" t="s">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="F52" s="1"/>
     </row>
@@ -2407,11 +2420,11 @@
         <v>392</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F53" s="1"/>
     </row>
@@ -2420,11 +2433,11 @@
         <v>392</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3" t="s">
-        <v>394</v>
+        <v>62</v>
       </c>
       <c r="F54" s="1"/>
     </row>
@@ -2433,11 +2446,11 @@
         <v>392</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F55" s="1"/>
     </row>
@@ -2446,11 +2459,11 @@
         <v>392</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F56" s="1"/>
     </row>
@@ -2459,11 +2472,11 @@
         <v>392</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F57" s="1"/>
     </row>
@@ -2472,11 +2485,11 @@
         <v>392</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3" t="s">
-        <v>67</v>
+        <v>397</v>
       </c>
       <c r="F58" s="1"/>
     </row>
@@ -2485,11 +2498,11 @@
         <v>392</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3" t="s">
-        <v>398</v>
+        <v>67</v>
       </c>
       <c r="F59" s="1"/>
     </row>
@@ -2498,39 +2511,39 @@
         <v>392</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>156</v>
-      </c>
+        <v>398</v>
+      </c>
+      <c r="F60" s="1"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>68</v>
+        <v>154</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>181</v>
+        <v>68</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
       <c r="F62" s="1"/>
     </row>
@@ -2539,11 +2552,11 @@
         <v>392</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3" t="s">
-        <v>71</v>
+        <v>182</v>
       </c>
       <c r="F63" s="1"/>
     </row>
@@ -2552,11 +2565,11 @@
         <v>392</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F64" s="1"/>
     </row>
@@ -2565,11 +2578,11 @@
         <v>392</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F65" s="1"/>
     </row>
@@ -2578,39 +2591,39 @@
         <v>392</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>77</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F66" s="1"/>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>183</v>
+        <v>76</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F67" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F68" s="1"/>
     </row>
@@ -2619,11 +2632,11 @@
         <v>392</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F69" s="1"/>
     </row>
@@ -2632,11 +2645,11 @@
         <v>392</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F70" s="1"/>
     </row>
@@ -2645,11 +2658,11 @@
         <v>392</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F71" s="1"/>
     </row>
@@ -2658,11 +2671,11 @@
         <v>392</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F72" s="1"/>
     </row>
@@ -2671,11 +2684,11 @@
         <v>392</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F73" s="1"/>
     </row>
@@ -2684,11 +2697,11 @@
         <v>392</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>78</v>
+        <v>195</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3" t="s">
-        <v>79</v>
+        <v>196</v>
       </c>
       <c r="F74" s="1"/>
     </row>
@@ -2697,11 +2710,11 @@
         <v>392</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F75" s="1"/>
     </row>
@@ -2710,11 +2723,11 @@
         <v>392</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>197</v>
+        <v>80</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
       <c r="F76" s="1"/>
     </row>
@@ -2723,11 +2736,11 @@
         <v>392</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="F77" s="1"/>
     </row>
@@ -2736,11 +2749,11 @@
         <v>392</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F78" s="1"/>
     </row>
@@ -2749,11 +2762,11 @@
         <v>392</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="F79" s="1"/>
     </row>
@@ -2762,11 +2775,11 @@
         <v>392</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>202</v>
+        <v>82</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3" t="s">
-        <v>203</v>
+        <v>83</v>
       </c>
       <c r="F80" s="1"/>
     </row>
@@ -2775,11 +2788,11 @@
         <v>392</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
       <c r="F81" s="1"/>
     </row>
@@ -2788,11 +2801,11 @@
         <v>392</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>204</v>
+        <v>84</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="F82" s="1"/>
     </row>
@@ -2801,11 +2814,11 @@
         <v>392</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F83" s="1"/>
     </row>
@@ -2814,11 +2827,11 @@
         <v>392</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>207</v>
+        <v>86</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F84" s="1"/>
     </row>
@@ -2827,11 +2840,11 @@
         <v>392</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3" t="s">
-        <v>113</v>
+        <v>208</v>
       </c>
       <c r="F85" s="1"/>
     </row>
@@ -2840,11 +2853,11 @@
         <v>392</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3" t="s">
-        <v>211</v>
+        <v>113</v>
       </c>
       <c r="F86" s="1"/>
     </row>
@@ -2853,11 +2866,11 @@
         <v>392</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F87" s="1"/>
     </row>
@@ -2866,11 +2879,11 @@
         <v>392</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F88" s="1"/>
     </row>
@@ -2879,11 +2892,11 @@
         <v>392</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F89" s="1"/>
     </row>
@@ -2892,11 +2905,11 @@
         <v>392</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3" t="s">
-        <v>58</v>
+        <v>217</v>
       </c>
       <c r="F90" s="1"/>
     </row>
@@ -2905,11 +2918,11 @@
         <v>392</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>87</v>
+        <v>218</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="F91" s="1"/>
     </row>
@@ -2918,11 +2931,11 @@
         <v>392</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F92" s="1"/>
     </row>
@@ -2931,11 +2944,11 @@
         <v>392</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>219</v>
+        <v>89</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3" t="s">
-        <v>220</v>
+        <v>90</v>
       </c>
       <c r="F93" s="1"/>
     </row>
@@ -2944,11 +2957,11 @@
         <v>392</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>91</v>
+        <v>219</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3" t="s">
-        <v>92</v>
+        <v>220</v>
       </c>
       <c r="F94" s="1"/>
     </row>
@@ -2957,11 +2970,11 @@
         <v>392</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>221</v>
+        <v>91</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3" t="s">
-        <v>222</v>
+        <v>92</v>
       </c>
       <c r="F95" s="1"/>
     </row>
@@ -2970,11 +2983,11 @@
         <v>392</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F96" s="1"/>
     </row>
@@ -2983,11 +2996,11 @@
         <v>392</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F97" s="1"/>
     </row>
@@ -2996,11 +3009,11 @@
         <v>392</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F98" s="1"/>
     </row>
@@ -3009,11 +3022,11 @@
         <v>392</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F99" s="1"/>
     </row>
@@ -3022,11 +3035,11 @@
         <v>392</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F100" s="1"/>
     </row>
@@ -3035,11 +3048,11 @@
         <v>392</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F101" s="1"/>
     </row>
@@ -3048,37 +3061,37 @@
         <v>392</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B104" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D104" s="3"/>
       <c r="E104" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F104" s="1"/>
     </row>
@@ -3087,11 +3100,11 @@
         <v>392</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D105" s="3"/>
       <c r="E105" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F105" s="1"/>
     </row>
@@ -3100,37 +3113,37 @@
         <v>392</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D108" s="3"/>
       <c r="E108" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F108" s="1"/>
     </row>
@@ -3139,11 +3152,11 @@
         <v>392</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F109" s="1"/>
     </row>
@@ -3152,11 +3165,11 @@
         <v>392</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F110" s="1"/>
     </row>
@@ -3165,76 +3178,76 @@
         <v>392</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D111" s="3"/>
       <c r="E111" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F116" s="1"/>
     </row>
@@ -3243,24 +3256,24 @@
         <v>392</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D117" s="3"/>
       <c r="E117" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D118" s="3"/>
       <c r="E118" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F118" s="1"/>
     </row>
@@ -3269,50 +3282,50 @@
         <v>392</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D119" s="3"/>
       <c r="E119" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F122" s="1"/>
     </row>
@@ -3321,167 +3334,167 @@
         <v>392</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>93</v>
+        <v>277</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3" t="s">
-        <v>94</v>
+        <v>278</v>
       </c>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>279</v>
+        <v>95</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3" t="s">
-        <v>280</v>
+        <v>96</v>
       </c>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3" t="s">
-        <v>30</v>
+        <v>280</v>
       </c>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3" t="s">
-        <v>283</v>
+        <v>30</v>
       </c>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>97</v>
+        <v>284</v>
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D131" s="3"/>
       <c r="E131" s="3" t="s">
-        <v>99</v>
+        <v>286</v>
       </c>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>287</v>
+        <v>98</v>
       </c>
       <c r="D132" s="3"/>
       <c r="E132" s="3" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D133" s="3"/>
       <c r="E133" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D134" s="3"/>
       <c r="E134" s="3" t="s">
-        <v>290</v>
+        <v>30</v>
       </c>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D135" s="3"/>
       <c r="E135" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F135" s="1"/>
     </row>
@@ -3490,24 +3503,24 @@
         <v>392</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>100</v>
+        <v>291</v>
       </c>
       <c r="D136" s="3"/>
       <c r="E136" s="3" t="s">
-        <v>101</v>
+        <v>292</v>
       </c>
       <c r="F136" s="1"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D137" s="3"/>
       <c r="E137" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F137" s="1"/>
     </row>
@@ -3516,11 +3529,11 @@
         <v>392</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D138" s="3"/>
       <c r="E138" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F138" s="1"/>
     </row>
@@ -3529,37 +3542,37 @@
         <v>392</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D139" s="3"/>
       <c r="E139" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>293</v>
+        <v>106</v>
       </c>
       <c r="D140" s="3"/>
       <c r="E140" s="3" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D141" s="3"/>
       <c r="E141" s="3" t="s">
-        <v>295</v>
+        <v>24</v>
       </c>
       <c r="F141" s="1"/>
     </row>
@@ -3568,11 +3581,11 @@
         <v>392</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D142" s="3"/>
       <c r="E142" s="3" t="s">
-        <v>108</v>
+        <v>295</v>
       </c>
       <c r="F142" s="1"/>
     </row>
@@ -3581,63 +3594,63 @@
         <v>392</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D143" s="3"/>
       <c r="E143" s="3" t="s">
-        <v>298</v>
+        <v>108</v>
       </c>
       <c r="F143" s="1"/>
     </row>
-    <row r="144" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D144" s="3"/>
       <c r="E144" s="3" t="s">
-        <v>109</v>
+        <v>298</v>
       </c>
       <c r="F144" s="1"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D145" s="3"/>
       <c r="E145" s="3" t="s">
-        <v>301</v>
+        <v>109</v>
       </c>
       <c r="F145" s="1"/>
     </row>
-    <row r="146" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>110</v>
+        <v>300</v>
       </c>
       <c r="D146" s="3"/>
       <c r="E146" s="3" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D147" s="3"/>
       <c r="E147" s="3" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="F147" s="1"/>
     </row>
@@ -3646,11 +3659,11 @@
         <v>392</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>303</v>
+        <v>111</v>
       </c>
       <c r="D148" s="3"/>
       <c r="E148" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F148" s="1"/>
     </row>
@@ -3659,11 +3672,11 @@
         <v>392</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D149" s="3"/>
       <c r="E149" s="3" t="s">
-        <v>112</v>
+        <v>304</v>
       </c>
       <c r="F149" s="1"/>
     </row>
@@ -3672,11 +3685,11 @@
         <v>392</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D150" s="3"/>
       <c r="E150" s="3" t="s">
-        <v>307</v>
+        <v>112</v>
       </c>
       <c r="F150" s="1"/>
     </row>
@@ -3685,11 +3698,11 @@
         <v>392</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D151" s="3"/>
       <c r="E151" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F151" s="1"/>
     </row>
@@ -3698,11 +3711,11 @@
         <v>392</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D152" s="3"/>
       <c r="E152" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F152" s="1"/>
     </row>
@@ -3711,11 +3724,11 @@
         <v>392</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D153" s="3"/>
       <c r="E153" s="3" t="s">
-        <v>112</v>
+        <v>311</v>
       </c>
       <c r="F153" s="1"/>
     </row>
@@ -3724,11 +3737,11 @@
         <v>392</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D154" s="3"/>
       <c r="E154" s="3" t="s">
-        <v>314</v>
+        <v>112</v>
       </c>
       <c r="F154" s="1"/>
     </row>
@@ -3737,11 +3750,11 @@
         <v>392</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D155" s="3"/>
       <c r="E155" s="3" t="s">
-        <v>180</v>
+        <v>314</v>
       </c>
       <c r="F155" s="1"/>
     </row>
@@ -3750,11 +3763,11 @@
         <v>392</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D156" s="3"/>
       <c r="E156" s="3" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="F156" s="1"/>
     </row>
@@ -3763,11 +3776,11 @@
         <v>392</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D157" s="3"/>
       <c r="E157" s="3" t="s">
-        <v>307</v>
+        <v>112</v>
       </c>
       <c r="F157" s="1"/>
     </row>
@@ -3776,11 +3789,11 @@
         <v>392</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>114</v>
+        <v>317</v>
       </c>
       <c r="D158" s="3"/>
       <c r="E158" s="3" t="s">
-        <v>115</v>
+        <v>307</v>
       </c>
       <c r="F158" s="1"/>
     </row>
@@ -3789,11 +3802,11 @@
         <v>392</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D159" s="3"/>
       <c r="E159" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F159" s="1"/>
     </row>
@@ -3802,11 +3815,11 @@
         <v>392</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>318</v>
+        <v>116</v>
       </c>
       <c r="D160" s="3"/>
       <c r="E160" s="3" t="s">
-        <v>319</v>
+        <v>117</v>
       </c>
       <c r="F160" s="1"/>
     </row>
@@ -3815,11 +3828,11 @@
         <v>392</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D161" s="3"/>
       <c r="E161" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F161" s="1"/>
     </row>
@@ -3828,24 +3841,24 @@
         <v>392</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>118</v>
+        <v>320</v>
       </c>
       <c r="D162" s="3"/>
       <c r="E162" s="3" t="s">
-        <v>71</v>
+        <v>321</v>
       </c>
       <c r="F162" s="1"/>
     </row>
-    <row r="163" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D163" s="3"/>
       <c r="E163" s="3" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="F163" s="1"/>
     </row>
@@ -3854,11 +3867,11 @@
         <v>392</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D164" s="3"/>
       <c r="E164" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F164" s="1"/>
     </row>
@@ -3867,76 +3880,76 @@
         <v>392</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D165" s="3"/>
       <c r="E165" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F165" s="1"/>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D166" s="3"/>
       <c r="E166" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F166" s="1"/>
     </row>
-    <row r="167" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D167" s="3"/>
       <c r="E167" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F167" s="1"/>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D168" s="3"/>
       <c r="E168" s="3" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="F168" s="1"/>
     </row>
-    <row r="169" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B169" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D169" s="3"/>
       <c r="E169" s="3" t="s">
-        <v>322</v>
+        <v>96</v>
       </c>
       <c r="F169" s="1"/>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D170" s="3"/>
       <c r="E170" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F170" s="1"/>
     </row>
@@ -3945,11 +3958,11 @@
         <v>392</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>324</v>
+        <v>131</v>
       </c>
       <c r="D171" s="3"/>
       <c r="E171" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F171" s="1"/>
     </row>
@@ -3958,11 +3971,11 @@
         <v>392</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D172" s="3"/>
       <c r="E172" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F172" s="1"/>
     </row>
@@ -3971,11 +3984,11 @@
         <v>392</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D173" s="3"/>
       <c r="E173" s="3" t="s">
-        <v>192</v>
+        <v>327</v>
       </c>
       <c r="F173" s="1"/>
     </row>
@@ -3984,11 +3997,11 @@
         <v>392</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D174" s="3"/>
       <c r="E174" s="3" t="s">
-        <v>330</v>
+        <v>192</v>
       </c>
       <c r="F174" s="1"/>
     </row>
@@ -3997,11 +4010,11 @@
         <v>392</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>132</v>
+        <v>329</v>
       </c>
       <c r="D175" s="3"/>
       <c r="E175" s="3" t="s">
-        <v>133</v>
+        <v>330</v>
       </c>
       <c r="F175" s="1"/>
     </row>
@@ -4010,11 +4023,11 @@
         <v>392</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>331</v>
+        <v>132</v>
       </c>
       <c r="D176" s="3"/>
       <c r="E176" s="3" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="F176" s="1"/>
     </row>
@@ -4023,11 +4036,11 @@
         <v>392</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D177" s="3"/>
       <c r="E177" s="3" t="s">
-        <v>333</v>
+        <v>171</v>
       </c>
       <c r="F177" s="1"/>
     </row>
@@ -4036,11 +4049,11 @@
         <v>392</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D178" s="3"/>
       <c r="E178" s="3" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="F178" s="1"/>
     </row>
@@ -4049,11 +4062,11 @@
         <v>392</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D179" s="3"/>
       <c r="E179" s="3" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="F179" s="1"/>
     </row>
@@ -4062,11 +4075,11 @@
         <v>392</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D180" s="3"/>
       <c r="E180" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F180" s="1"/>
     </row>
@@ -4075,11 +4088,11 @@
         <v>392</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D181" s="3"/>
       <c r="E181" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F181" s="1"/>
     </row>
@@ -4088,114 +4101,114 @@
         <v>392</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D182" s="3"/>
       <c r="E182" s="3" t="s">
-        <v>173</v>
+        <v>340</v>
       </c>
       <c r="F182" s="1"/>
-      <c r="N182" s="2"/>
-      <c r="P182" s="2"/>
     </row>
     <row r="183" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B183" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D183" s="3"/>
       <c r="E183" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F183" s="1"/>
+      <c r="N183" s="2"/>
+      <c r="P183" s="2"/>
     </row>
     <row r="184" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B184" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D184" s="3"/>
       <c r="E184" s="3" t="s">
-        <v>344</v>
+        <v>175</v>
       </c>
       <c r="F184" s="1"/>
-      <c r="H184" s="2"/>
-      <c r="N184" s="2"/>
-      <c r="P184" s="2"/>
-      <c r="V184" s="2"/>
-      <c r="X184" s="2"/>
-      <c r="Z184" s="2"/>
-      <c r="AB184" s="2"/>
-      <c r="AD184" s="2"/>
-      <c r="AF184" s="2"/>
     </row>
     <row r="185" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B185" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D185" s="3"/>
       <c r="E185" s="3" t="s">
         <v>344</v>
       </c>
       <c r="F185" s="1"/>
+      <c r="H185" s="2"/>
+      <c r="N185" s="2"/>
+      <c r="P185" s="2"/>
+      <c r="V185" s="2"/>
+      <c r="X185" s="2"/>
+      <c r="Z185" s="2"/>
+      <c r="AB185" s="2"/>
+      <c r="AD185" s="2"/>
+      <c r="AF185" s="2"/>
     </row>
     <row r="186" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B186" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D186" s="3"/>
       <c r="E186" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F186" s="1"/>
-      <c r="H186" s="2"/>
-      <c r="J186" s="2"/>
-      <c r="L186" s="2"/>
-      <c r="N186" s="2"/>
-      <c r="P186" s="2"/>
-      <c r="R186" s="2"/>
-      <c r="T186" s="2"/>
-      <c r="V186" s="2"/>
-      <c r="X186" s="2"/>
-      <c r="Z186" s="2"/>
-      <c r="AB186" s="2"/>
-      <c r="AD186" s="2"/>
-      <c r="AF186" s="2"/>
-      <c r="AH186" s="2"/>
     </row>
     <row r="187" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B187" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>134</v>
+        <v>346</v>
       </c>
       <c r="D187" s="3"/>
       <c r="E187" s="3" t="s">
-        <v>135</v>
+        <v>347</v>
       </c>
       <c r="F187" s="1"/>
+      <c r="H187" s="2"/>
+      <c r="J187" s="2"/>
+      <c r="L187" s="2"/>
+      <c r="N187" s="2"/>
+      <c r="P187" s="2"/>
+      <c r="R187" s="2"/>
+      <c r="T187" s="2"/>
+      <c r="V187" s="2"/>
+      <c r="X187" s="2"/>
+      <c r="Z187" s="2"/>
+      <c r="AB187" s="2"/>
+      <c r="AD187" s="2"/>
+      <c r="AF187" s="2"/>
+      <c r="AH187" s="2"/>
     </row>
     <row r="188" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B188" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>348</v>
+        <v>134</v>
       </c>
       <c r="D188" s="3"/>
       <c r="E188" s="3" t="s">
-        <v>349</v>
+        <v>135</v>
       </c>
       <c r="F188" s="1"/>
     </row>
@@ -4204,11 +4217,11 @@
         <v>392</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>136</v>
+        <v>348</v>
       </c>
       <c r="D189" s="3"/>
       <c r="E189" s="3" t="s">
-        <v>137</v>
+        <v>349</v>
       </c>
       <c r="F189" s="1"/>
     </row>
@@ -4217,11 +4230,11 @@
         <v>392</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>350</v>
+        <v>136</v>
       </c>
       <c r="D190" s="3"/>
       <c r="E190" s="3" t="s">
-        <v>351</v>
+        <v>137</v>
       </c>
       <c r="F190" s="1"/>
     </row>
@@ -4230,11 +4243,11 @@
         <v>392</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D191" s="3"/>
       <c r="E191" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F191" s="1"/>
     </row>
@@ -4243,11 +4256,11 @@
         <v>392</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>138</v>
+        <v>352</v>
       </c>
       <c r="D192" s="3"/>
       <c r="E192" s="3" t="s">
-        <v>139</v>
+        <v>353</v>
       </c>
       <c r="F192" s="1"/>
     </row>
@@ -4256,11 +4269,11 @@
         <v>392</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D193" s="3"/>
       <c r="E193" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F193" s="1"/>
     </row>
@@ -4269,11 +4282,11 @@
         <v>392</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>354</v>
+        <v>140</v>
       </c>
       <c r="D194" s="3"/>
       <c r="E194" s="3" t="s">
-        <v>355</v>
+        <v>141</v>
       </c>
       <c r="F194" s="1"/>
     </row>
@@ -4282,11 +4295,11 @@
         <v>392</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>142</v>
+        <v>354</v>
       </c>
       <c r="D195" s="3"/>
       <c r="E195" s="3" t="s">
-        <v>73</v>
+        <v>355</v>
       </c>
       <c r="F195" s="1"/>
     </row>
@@ -4295,11 +4308,11 @@
         <v>392</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D196" s="3"/>
       <c r="E196" s="3" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="F196" s="1"/>
     </row>
@@ -4308,11 +4321,11 @@
         <v>392</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>356</v>
+        <v>143</v>
       </c>
       <c r="D197" s="3"/>
       <c r="E197" s="3" t="s">
-        <v>357</v>
+        <v>144</v>
       </c>
       <c r="F197" s="1"/>
     </row>
@@ -4321,11 +4334,11 @@
         <v>392</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D198" s="3"/>
       <c r="E198" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F198" s="1"/>
     </row>
@@ -4334,11 +4347,11 @@
         <v>392</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>145</v>
+        <v>358</v>
       </c>
       <c r="D199" s="3"/>
       <c r="E199" s="3" t="s">
-        <v>146</v>
+        <v>359</v>
       </c>
       <c r="F199" s="1"/>
     </row>
@@ -4347,178 +4360,174 @@
         <v>392</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D200" s="3"/>
       <c r="E200" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F200" s="1"/>
-      <c r="L200" s="2"/>
-      <c r="N200" s="2"/>
-      <c r="P200" s="2"/>
-      <c r="V200" s="2"/>
-      <c r="X200" s="2"/>
-      <c r="Z200" s="2"/>
     </row>
     <row r="201" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B201" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>360</v>
+        <v>147</v>
       </c>
       <c r="D201" s="3"/>
       <c r="E201" s="3" t="s">
-        <v>361</v>
+        <v>148</v>
       </c>
       <c r="F201" s="1"/>
+      <c r="L201" s="2"/>
+      <c r="N201" s="2"/>
+      <c r="P201" s="2"/>
+      <c r="V201" s="2"/>
+      <c r="X201" s="2"/>
+      <c r="Z201" s="2"/>
     </row>
     <row r="202" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B202" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>149</v>
+        <v>360</v>
       </c>
       <c r="D202" s="3"/>
       <c r="E202" s="3" t="s">
-        <v>150</v>
+        <v>361</v>
       </c>
       <c r="F202" s="1"/>
-      <c r="H202" s="2"/>
-      <c r="J202" s="2"/>
-      <c r="L202" s="2"/>
-      <c r="N202" s="2"/>
-      <c r="P202" s="2"/>
-      <c r="R202" s="2"/>
-      <c r="T202" s="2"/>
-      <c r="V202" s="2"/>
-      <c r="X202" s="2"/>
-      <c r="Z202" s="2"/>
-      <c r="AB202" s="2"/>
     </row>
     <row r="203" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B203" s="1" t="s">
         <v>392</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D203" s="3"/>
       <c r="E203" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F203" s="1"/>
+      <c r="H203" s="2"/>
+      <c r="J203" s="2"/>
+      <c r="L203" s="2"/>
+      <c r="N203" s="2"/>
+      <c r="P203" s="2"/>
+      <c r="R203" s="2"/>
+      <c r="T203" s="2"/>
+      <c r="V203" s="2"/>
+      <c r="X203" s="2"/>
+      <c r="Z203" s="2"/>
+      <c r="AB203" s="2"/>
+    </row>
+    <row r="204" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B204" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D204" s="3"/>
+      <c r="E204" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F203" s="1"/>
-    </row>
-    <row r="229" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F229" s="2"/>
-      <c r="H229" s="2"/>
-      <c r="J229" s="2"/>
-      <c r="L229" s="2"/>
-      <c r="N229" s="2"/>
-      <c r="P229" s="2"/>
-      <c r="R229" s="2"/>
-      <c r="T229" s="2"/>
-      <c r="X229" s="2"/>
-      <c r="Z229" s="2"/>
-      <c r="AB229" s="2"/>
-      <c r="AD229" s="2"/>
-      <c r="AF229" s="2"/>
-      <c r="AH229" s="2"/>
-    </row>
-    <row r="231" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F231" s="2"/>
-      <c r="H231" s="2"/>
-      <c r="J231" s="2"/>
-      <c r="L231" s="2"/>
-      <c r="N231" s="2"/>
-      <c r="P231" s="2"/>
-      <c r="R231" s="2"/>
-      <c r="T231" s="2"/>
-      <c r="V231" s="2"/>
-      <c r="X231" s="2"/>
-      <c r="Z231" s="2"/>
-      <c r="AB231" s="2"/>
-      <c r="AD231" s="2"/>
-      <c r="AF231" s="2"/>
-      <c r="AH231" s="2"/>
-    </row>
-    <row r="233" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F233" s="2"/>
-      <c r="H233" s="2"/>
-      <c r="J233" s="2"/>
-      <c r="L233" s="2"/>
-      <c r="N233" s="2"/>
-      <c r="P233" s="2"/>
-      <c r="R233" s="2"/>
-      <c r="T233" s="2"/>
-      <c r="V233" s="2"/>
-      <c r="X233" s="2"/>
-      <c r="Z233" s="2"/>
-      <c r="AB233" s="2"/>
-      <c r="AD233" s="2"/>
-      <c r="AF233" s="2"/>
-      <c r="AH233" s="2"/>
-    </row>
-    <row r="235" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F235" s="2"/>
-      <c r="H235" s="2"/>
-      <c r="J235" s="2"/>
-      <c r="L235" s="2"/>
-      <c r="N235" s="2"/>
-      <c r="P235" s="2"/>
-      <c r="X235" s="2"/>
-      <c r="AB235" s="2"/>
-      <c r="AD235" s="2"/>
-      <c r="AF235" s="2"/>
-    </row>
-    <row r="237" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F237" s="2"/>
-      <c r="H237" s="2"/>
-      <c r="J237" s="2"/>
-      <c r="L237" s="2"/>
-      <c r="N237" s="2"/>
-      <c r="P237" s="2"/>
-      <c r="R237" s="2"/>
-      <c r="T237" s="2"/>
-      <c r="X237" s="2"/>
-      <c r="Z237" s="2"/>
-      <c r="AB237" s="2"/>
-      <c r="AD237" s="2"/>
-      <c r="AF237" s="2"/>
-      <c r="AH237" s="2"/>
-    </row>
-    <row r="243" spans="6:32" x14ac:dyDescent="0.25">
-      <c r="F243" s="2"/>
-      <c r="H243" s="2"/>
-      <c r="J243" s="2"/>
-      <c r="L243" s="2"/>
-      <c r="N243" s="2"/>
-      <c r="P243" s="2"/>
-      <c r="V243" s="2"/>
-      <c r="X243" s="2"/>
-      <c r="Z243" s="2"/>
-      <c r="AB243" s="2"/>
-      <c r="AD243" s="2"/>
-      <c r="AF243" s="2"/>
-    </row>
-    <row r="273" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F273" s="2"/>
-      <c r="H273" s="2"/>
-      <c r="J273" s="2"/>
-      <c r="L273" s="2"/>
-      <c r="N273" s="2"/>
-      <c r="P273" s="2"/>
-      <c r="R273" s="2"/>
-      <c r="T273" s="2"/>
-      <c r="V273" s="2"/>
-      <c r="X273" s="2"/>
-      <c r="Z273" s="2"/>
-      <c r="AB273" s="2"/>
-      <c r="AD273" s="2"/>
-      <c r="AF273" s="2"/>
-      <c r="AH273" s="2"/>
+      <c r="F204" s="1"/>
+    </row>
+    <row r="230" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="F230" s="2"/>
+      <c r="H230" s="2"/>
+      <c r="J230" s="2"/>
+      <c r="L230" s="2"/>
+      <c r="N230" s="2"/>
+      <c r="P230" s="2"/>
+      <c r="R230" s="2"/>
+      <c r="T230" s="2"/>
+      <c r="X230" s="2"/>
+      <c r="Z230" s="2"/>
+      <c r="AB230" s="2"/>
+      <c r="AD230" s="2"/>
+      <c r="AF230" s="2"/>
+      <c r="AH230" s="2"/>
+    </row>
+    <row r="232" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="F232" s="2"/>
+      <c r="H232" s="2"/>
+      <c r="J232" s="2"/>
+      <c r="L232" s="2"/>
+      <c r="N232" s="2"/>
+      <c r="P232" s="2"/>
+      <c r="R232" s="2"/>
+      <c r="T232" s="2"/>
+      <c r="V232" s="2"/>
+      <c r="X232" s="2"/>
+      <c r="Z232" s="2"/>
+      <c r="AB232" s="2"/>
+      <c r="AD232" s="2"/>
+      <c r="AF232" s="2"/>
+      <c r="AH232" s="2"/>
+    </row>
+    <row r="234" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="F234" s="2"/>
+      <c r="H234" s="2"/>
+      <c r="J234" s="2"/>
+      <c r="L234" s="2"/>
+      <c r="N234" s="2"/>
+      <c r="P234" s="2"/>
+      <c r="R234" s="2"/>
+      <c r="T234" s="2"/>
+      <c r="V234" s="2"/>
+      <c r="X234" s="2"/>
+      <c r="Z234" s="2"/>
+      <c r="AB234" s="2"/>
+      <c r="AD234" s="2"/>
+      <c r="AF234" s="2"/>
+      <c r="AH234" s="2"/>
+    </row>
+    <row r="236" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="F236" s="2"/>
+      <c r="H236" s="2"/>
+      <c r="J236" s="2"/>
+      <c r="L236" s="2"/>
+      <c r="N236" s="2"/>
+      <c r="P236" s="2"/>
+      <c r="X236" s="2"/>
+      <c r="AB236" s="2"/>
+      <c r="AD236" s="2"/>
+      <c r="AF236" s="2"/>
+    </row>
+    <row r="238" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="F238" s="2"/>
+      <c r="H238" s="2"/>
+      <c r="J238" s="2"/>
+      <c r="L238" s="2"/>
+      <c r="N238" s="2"/>
+      <c r="P238" s="2"/>
+      <c r="R238" s="2"/>
+      <c r="T238" s="2"/>
+      <c r="X238" s="2"/>
+      <c r="Z238" s="2"/>
+      <c r="AB238" s="2"/>
+      <c r="AD238" s="2"/>
+      <c r="AF238" s="2"/>
+      <c r="AH238" s="2"/>
+    </row>
+    <row r="244" spans="6:32" x14ac:dyDescent="0.25">
+      <c r="F244" s="2"/>
+      <c r="H244" s="2"/>
+      <c r="J244" s="2"/>
+      <c r="L244" s="2"/>
+      <c r="N244" s="2"/>
+      <c r="P244" s="2"/>
+      <c r="V244" s="2"/>
+      <c r="X244" s="2"/>
+      <c r="Z244" s="2"/>
+      <c r="AB244" s="2"/>
+      <c r="AD244" s="2"/>
+      <c r="AF244" s="2"/>
     </row>
     <row r="274" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F274" s="2"/>
@@ -4537,12 +4546,22 @@
       <c r="AF274" s="2"/>
       <c r="AH274" s="2"/>
     </row>
-    <row r="280" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="N280" s="2"/>
-      <c r="P280" s="2"/>
-      <c r="V280" s="2"/>
-      <c r="X280" s="2"/>
-      <c r="Z280" s="2"/>
+    <row r="275" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="F275" s="2"/>
+      <c r="H275" s="2"/>
+      <c r="J275" s="2"/>
+      <c r="L275" s="2"/>
+      <c r="N275" s="2"/>
+      <c r="P275" s="2"/>
+      <c r="R275" s="2"/>
+      <c r="T275" s="2"/>
+      <c r="V275" s="2"/>
+      <c r="X275" s="2"/>
+      <c r="Z275" s="2"/>
+      <c r="AB275" s="2"/>
+      <c r="AD275" s="2"/>
+      <c r="AF275" s="2"/>
+      <c r="AH275" s="2"/>
     </row>
     <row r="281" spans="6:34" x14ac:dyDescent="0.25">
       <c r="N281" s="2"/>
@@ -4551,126 +4570,127 @@
       <c r="X281" s="2"/>
       <c r="Z281" s="2"/>
     </row>
-    <row r="284" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="N284" s="2"/>
-      <c r="P284" s="2"/>
-      <c r="V284" s="2"/>
-      <c r="X284" s="2"/>
-      <c r="Z284" s="2"/>
-    </row>
-    <row r="288" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="N288" s="2"/>
-      <c r="P288" s="2"/>
-      <c r="V288" s="2"/>
-      <c r="X288" s="2"/>
-      <c r="Z288" s="2"/>
-    </row>
-    <row r="292" spans="6:28" x14ac:dyDescent="0.25">
-      <c r="F292" s="2"/>
-      <c r="H292" s="2"/>
-      <c r="J292" s="2"/>
-      <c r="L292" s="2"/>
-      <c r="N292" s="2"/>
-      <c r="P292" s="2"/>
-      <c r="R292" s="2"/>
-      <c r="T292" s="2"/>
-      <c r="V292" s="2"/>
-      <c r="X292" s="2"/>
-      <c r="Z292" s="2"/>
-      <c r="AB292" s="2"/>
-    </row>
-    <row r="296" spans="6:28" x14ac:dyDescent="0.25">
-      <c r="L296" s="2"/>
-      <c r="N296" s="2"/>
-      <c r="P296" s="2"/>
-      <c r="V296" s="2"/>
-      <c r="X296" s="2"/>
-      <c r="Z296" s="2"/>
-    </row>
-    <row r="298" spans="6:28" x14ac:dyDescent="0.25">
-      <c r="F298" s="2"/>
-      <c r="H298" s="2"/>
-      <c r="J298" s="2"/>
-      <c r="L298" s="2"/>
-      <c r="N298" s="2"/>
-      <c r="P298" s="2"/>
-      <c r="R298" s="2"/>
-      <c r="T298" s="2"/>
-      <c r="V298" s="2"/>
-      <c r="X298" s="2"/>
-      <c r="Z298" s="2"/>
-      <c r="AB298" s="2"/>
-    </row>
-    <row r="300" spans="6:28" x14ac:dyDescent="0.25">
-      <c r="F300" s="2"/>
-      <c r="H300" s="2"/>
-      <c r="J300" s="2"/>
-      <c r="L300" s="2"/>
-      <c r="N300" s="2"/>
-      <c r="P300" s="2"/>
-      <c r="R300" s="2"/>
-      <c r="T300" s="2"/>
-      <c r="V300" s="2"/>
-      <c r="X300" s="2"/>
-      <c r="Z300" s="2"/>
-      <c r="AB300" s="2"/>
-    </row>
-    <row r="302" spans="6:28" x14ac:dyDescent="0.25">
-      <c r="L302" s="2"/>
-      <c r="N302" s="2"/>
-      <c r="P302" s="2"/>
-      <c r="V302" s="2"/>
-      <c r="X302" s="2"/>
-      <c r="Z302" s="2"/>
-    </row>
-    <row r="304" spans="6:28" x14ac:dyDescent="0.25">
-      <c r="F304" s="2"/>
-      <c r="H304" s="2"/>
-      <c r="L304" s="2"/>
-      <c r="N304" s="2"/>
-      <c r="P304" s="2"/>
-      <c r="V304" s="2"/>
-      <c r="Z304" s="2"/>
-      <c r="AB304" s="2"/>
-    </row>
-    <row r="308" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F308" s="2"/>
-      <c r="H308" s="2"/>
-      <c r="L308" s="2"/>
-      <c r="N308" s="2"/>
-      <c r="P308" s="2"/>
-      <c r="V308" s="2"/>
-      <c r="X308" s="2"/>
-      <c r="Z308" s="2"/>
-      <c r="AB308" s="2"/>
-    </row>
-    <row r="310" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="P310" s="2"/>
-    </row>
-    <row r="312" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F312" s="2"/>
-      <c r="H312" s="2"/>
-      <c r="J312" s="2"/>
-      <c r="L312" s="2"/>
-      <c r="N312" s="2"/>
-      <c r="P312" s="2"/>
-      <c r="R312" s="2"/>
-      <c r="V312" s="2"/>
-      <c r="X312" s="2"/>
-      <c r="Z312" s="2"/>
-      <c r="AB312" s="2"/>
-    </row>
-    <row r="320" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="L320" s="2"/>
-      <c r="N320" s="2"/>
-      <c r="P320" s="2"/>
-      <c r="AH320" s="2"/>
-    </row>
-    <row r="323" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="L323" s="2"/>
-      <c r="N323" s="2"/>
-      <c r="P323" s="2"/>
-      <c r="AH323" s="2"/>
+    <row r="282" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="N282" s="2"/>
+      <c r="P282" s="2"/>
+      <c r="V282" s="2"/>
+      <c r="X282" s="2"/>
+      <c r="Z282" s="2"/>
+    </row>
+    <row r="285" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="N285" s="2"/>
+      <c r="P285" s="2"/>
+      <c r="V285" s="2"/>
+      <c r="X285" s="2"/>
+      <c r="Z285" s="2"/>
+    </row>
+    <row r="289" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="N289" s="2"/>
+      <c r="P289" s="2"/>
+      <c r="V289" s="2"/>
+      <c r="X289" s="2"/>
+      <c r="Z289" s="2"/>
+    </row>
+    <row r="293" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F293" s="2"/>
+      <c r="H293" s="2"/>
+      <c r="J293" s="2"/>
+      <c r="L293" s="2"/>
+      <c r="N293" s="2"/>
+      <c r="P293" s="2"/>
+      <c r="R293" s="2"/>
+      <c r="T293" s="2"/>
+      <c r="V293" s="2"/>
+      <c r="X293" s="2"/>
+      <c r="Z293" s="2"/>
+      <c r="AB293" s="2"/>
+    </row>
+    <row r="297" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="L297" s="2"/>
+      <c r="N297" s="2"/>
+      <c r="P297" s="2"/>
+      <c r="V297" s="2"/>
+      <c r="X297" s="2"/>
+      <c r="Z297" s="2"/>
+    </row>
+    <row r="299" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F299" s="2"/>
+      <c r="H299" s="2"/>
+      <c r="J299" s="2"/>
+      <c r="L299" s="2"/>
+      <c r="N299" s="2"/>
+      <c r="P299" s="2"/>
+      <c r="R299" s="2"/>
+      <c r="T299" s="2"/>
+      <c r="V299" s="2"/>
+      <c r="X299" s="2"/>
+      <c r="Z299" s="2"/>
+      <c r="AB299" s="2"/>
+    </row>
+    <row r="301" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F301" s="2"/>
+      <c r="H301" s="2"/>
+      <c r="J301" s="2"/>
+      <c r="L301" s="2"/>
+      <c r="N301" s="2"/>
+      <c r="P301" s="2"/>
+      <c r="R301" s="2"/>
+      <c r="T301" s="2"/>
+      <c r="V301" s="2"/>
+      <c r="X301" s="2"/>
+      <c r="Z301" s="2"/>
+      <c r="AB301" s="2"/>
+    </row>
+    <row r="303" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="L303" s="2"/>
+      <c r="N303" s="2"/>
+      <c r="P303" s="2"/>
+      <c r="V303" s="2"/>
+      <c r="X303" s="2"/>
+      <c r="Z303" s="2"/>
+    </row>
+    <row r="305" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F305" s="2"/>
+      <c r="H305" s="2"/>
+      <c r="L305" s="2"/>
+      <c r="N305" s="2"/>
+      <c r="P305" s="2"/>
+      <c r="V305" s="2"/>
+      <c r="Z305" s="2"/>
+      <c r="AB305" s="2"/>
+    </row>
+    <row r="309" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F309" s="2"/>
+      <c r="H309" s="2"/>
+      <c r="L309" s="2"/>
+      <c r="N309" s="2"/>
+      <c r="P309" s="2"/>
+      <c r="V309" s="2"/>
+      <c r="X309" s="2"/>
+      <c r="Z309" s="2"/>
+      <c r="AB309" s="2"/>
+    </row>
+    <row r="311" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="P311" s="2"/>
+    </row>
+    <row r="313" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F313" s="2"/>
+      <c r="H313" s="2"/>
+      <c r="J313" s="2"/>
+      <c r="L313" s="2"/>
+      <c r="N313" s="2"/>
+      <c r="P313" s="2"/>
+      <c r="R313" s="2"/>
+      <c r="V313" s="2"/>
+      <c r="X313" s="2"/>
+      <c r="Z313" s="2"/>
+      <c r="AB313" s="2"/>
+    </row>
+    <row r="321" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="L321" s="2"/>
+      <c r="N321" s="2"/>
+      <c r="P321" s="2"/>
+      <c r="AH321" s="2"/>
     </row>
     <row r="324" spans="6:34" x14ac:dyDescent="0.25">
       <c r="L324" s="2"/>
@@ -4678,25 +4698,17 @@
       <c r="P324" s="2"/>
       <c r="AH324" s="2"/>
     </row>
-    <row r="326" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="L326" s="2"/>
-      <c r="N326" s="2"/>
-      <c r="P326" s="2"/>
-      <c r="AH326" s="2"/>
-    </row>
-    <row r="331" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="F331" s="2"/>
-      <c r="H331" s="2"/>
-      <c r="J331" s="2"/>
-      <c r="L331" s="2"/>
-      <c r="N331" s="2"/>
-      <c r="P331" s="2"/>
-      <c r="R331" s="2"/>
-      <c r="T331" s="2"/>
-      <c r="V331" s="2"/>
-      <c r="X331" s="2"/>
-      <c r="Z331" s="2"/>
-      <c r="AB331" s="2"/>
+    <row r="325" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="L325" s="2"/>
+      <c r="N325" s="2"/>
+      <c r="P325" s="2"/>
+      <c r="AH325" s="2"/>
+    </row>
+    <row r="327" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="L327" s="2"/>
+      <c r="N327" s="2"/>
+      <c r="P327" s="2"/>
+      <c r="AH327" s="2"/>
     </row>
     <row r="332" spans="6:34" x14ac:dyDescent="0.25">
       <c r="F332" s="2"/>
@@ -4712,6 +4724,20 @@
       <c r="Z332" s="2"/>
       <c r="AB332" s="2"/>
     </row>
+    <row r="333" spans="6:34" x14ac:dyDescent="0.25">
+      <c r="F333" s="2"/>
+      <c r="H333" s="2"/>
+      <c r="J333" s="2"/>
+      <c r="L333" s="2"/>
+      <c r="N333" s="2"/>
+      <c r="P333" s="2"/>
+      <c r="R333" s="2"/>
+      <c r="T333" s="2"/>
+      <c r="V333" s="2"/>
+      <c r="X333" s="2"/>
+      <c r="Z333" s="2"/>
+      <c r="AB333" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>